<commit_message>
Added data to exp 4
</commit_message>
<xml_diff>
--- a/PlantTransTwo/PlantTransII_ExpIV.xlsx
+++ b/PlantTransTwo/PlantTransII_ExpIV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>Load</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -353,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,122 +383,170 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>145</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>146</v>
       </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
       <c r="C3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>147</v>
       </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>148</v>
       </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>149</v>
       </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>150</v>
       </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>151</v>
       </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>152</v>
       </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
       <c r="C9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>153</v>
       </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
       <c r="C10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>154</v>
       </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
       <c r="C11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>155</v>
       </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
       <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>156</v>
       </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
       <c r="C13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>157</v>
       </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
       <c r="C14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>158</v>
       </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
       <c r="C15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>159</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -499,6 +556,9 @@
       <c r="A17">
         <v>160</v>
       </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
       <c r="C17">
         <v>3</v>
       </c>
@@ -507,6 +567,9 @@
       <c r="A18">
         <v>161</v>
       </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
       <c r="C18">
         <v>3</v>
       </c>
@@ -515,6 +578,9 @@
       <c r="A19">
         <v>162</v>
       </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
       <c r="C19">
         <v>3</v>
       </c>
@@ -523,6 +589,9 @@
       <c r="A20">
         <v>163</v>
       </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
       <c r="C20">
         <v>3</v>
       </c>
@@ -531,6 +600,9 @@
       <c r="A21">
         <v>164</v>
       </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
       <c r="C21">
         <v>4</v>
       </c>
@@ -539,6 +611,9 @@
       <c r="A22">
         <v>165</v>
       </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
       <c r="C22">
         <v>4</v>
       </c>
@@ -547,6 +622,9 @@
       <c r="A23">
         <v>166</v>
       </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
       <c r="C23">
         <v>4</v>
       </c>
@@ -555,6 +633,9 @@
       <c r="A24">
         <v>167</v>
       </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
       <c r="C24">
         <v>4</v>
       </c>
@@ -563,6 +644,9 @@
       <c r="A25">
         <v>168</v>
       </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
       <c r="C25">
         <v>4</v>
       </c>
@@ -570,6 +654,9 @@
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>169</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
       </c>
       <c r="C26">
         <v>4</v>

</xml_diff>